<commit_message>
Orden archivo Limpieza data clusters
</commit_message>
<xml_diff>
--- a/centrales_faltante_eolico.xlsx
+++ b/centrales_faltante_eolico.xlsx
@@ -508,7 +508,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>PE VALLE DE LOS VIENTOS</t>
+          <t>PE ALENA</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -554,7 +554,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>PE LOS BUENOS AIRES</t>
+          <t>PE AURORA</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -600,7 +600,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>PE LEBU</t>
+          <t>PE CABO LEONES</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -646,7 +646,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>PE LA FLOR</t>
+          <t>PE CABO LEONES II</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -692,7 +692,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>PE LA ESTRELLA</t>
+          <t>PE CABO LEONES III</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -738,7 +738,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>PE LA ESPERANZA</t>
+          <t>PE CALAMA</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -784,35 +784,35 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>PE EL MAITEN</t>
+          <t>PE CAMPO LINDO</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K8" t="n">
         <v>0</v>
@@ -830,7 +830,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>PE EL ARRAYAN</t>
+          <t>PE CANELA</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -876,7 +876,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>PE CUEL</t>
+          <t>PE CANELA II</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -922,7 +922,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>PE CANELA II</t>
+          <t>PE CERRO TIGRE</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -968,7 +968,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>PE CANELA</t>
+          <t>PE CUEL</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -1014,7 +1014,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>PE CALAMA</t>
+          <t>PE EL ARRAYAN</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -1060,7 +1060,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>PE CABO LEONES III</t>
+          <t>PE EL MAITEN</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -1106,7 +1106,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>PE CABO LEONES II</t>
+          <t>PE LA ESPERANZA</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -1152,7 +1152,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>PE CABO LEONES</t>
+          <t>PE LA ESTRELLA</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -1198,7 +1198,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>PE AURORA</t>
+          <t>PE LA FLOR</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -1244,7 +1244,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>PE ALENA</t>
+          <t>PE LEBU</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -1290,32 +1290,32 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>PE UCUQUER II</t>
+          <t>PE LLANOS DEL VIENTO</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J19" t="n">
         <v>0</v>
@@ -1336,11 +1336,11 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>PE LOS CURUROS</t>
+          <t>PE LOMAS DE DUQUECO</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C20" t="n">
         <v>0</v>
@@ -1382,7 +1382,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>PE LOS OLMOS</t>
+          <t>PE LOS BUENOS AIRES</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -1428,7 +1428,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>PE CERRO TIGRE</t>
+          <t>PE LOS CURUROS</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -1474,7 +1474,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>PE MALLECO SUR</t>
+          <t>PE LOS OLMOS</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -1520,7 +1520,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>PE TOTORAL</t>
+          <t>PE MALLECO NORTE</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -1566,7 +1566,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>PE MALLECO NORTE</t>
+          <t>PE MALLECO SUR</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -1612,7 +1612,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>PE TOLPAN SUR</t>
+          <t>PE MESAMAVIDA</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -1658,7 +1658,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>PE TCHAMMA</t>
+          <t>PE MONTE REDONDO</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -1704,7 +1704,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>PE TALTAL</t>
+          <t>PE NEGRETE</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -1750,26 +1750,26 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>PE TALINAY PONIENTE</t>
+          <t>PE PUELCHE SUR</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C29" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D29" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E29" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F29" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G29" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H29" t="n">
         <v>0</v>
@@ -1796,7 +1796,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>PE SIERRA GORDA ESTE</t>
+          <t>PE PUNTA COLORADA</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -1842,7 +1842,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>PE SARCO</t>
+          <t>PE PUNTA PALMERAS</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -1888,7 +1888,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>PE SAN PEDRO II</t>
+          <t>PE PUNTA SIERRA</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -1934,7 +1934,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>PE TALINAY ORIENTE</t>
+          <t>PE RENAICO I</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -1980,7 +1980,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>PE SAN JUAN</t>
+          <t>PE SAN GABRIEL</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -2026,7 +2026,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>PE SAN GABRIEL</t>
+          <t>PE SAN JUAN</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -2072,17 +2072,17 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>PE RENAICO I</t>
+          <t>PE SAN PEDRO</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C36" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D36" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E36" t="n">
         <v>0</v>
@@ -2118,7 +2118,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>PE PUNTA SIERRA</t>
+          <t>PE SAN PEDRO II</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -2164,7 +2164,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>PE PUNTA PALMERAS</t>
+          <t>PE SARCO</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -2210,7 +2210,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>PE PUNTA COLORADA</t>
+          <t>PE SIERRA GORDA ESTE</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -2256,7 +2256,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>PE NEGRETE</t>
+          <t>PE TALINAY ORIENTE</t>
         </is>
       </c>
       <c r="B40" t="n">
@@ -2302,7 +2302,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>PE MONTE REDONDO</t>
+          <t>PE TALINAY PONIENTE</t>
         </is>
       </c>
       <c r="B41" t="n">
@@ -2348,7 +2348,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>PE MESAMAVIDA</t>
+          <t>PE TALTAL</t>
         </is>
       </c>
       <c r="B42" t="n">
@@ -2394,11 +2394,11 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>PE LOMAS DE DUQUECO</t>
+          <t>PE TCHAMMA</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C43" t="n">
         <v>0</v>
@@ -2440,17 +2440,17 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>PE SAN PEDRO</t>
+          <t>PE TOLPAN SUR</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C44" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D44" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E44" t="n">
         <v>0</v>
@@ -2486,26 +2486,26 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>PE PUELCHE SUR</t>
+          <t>PE TOTORAL</t>
         </is>
       </c>
       <c r="B45" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C45" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D45" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E45" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F45" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G45" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H45" t="n">
         <v>0</v>
@@ -2532,32 +2532,32 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>PE LLANOS DEL VIENTO</t>
+          <t>PE UCUQUER II</t>
         </is>
       </c>
       <c r="B46" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C46" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D46" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E46" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F46" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G46" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H46" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I46" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J46" t="n">
         <v>0</v>
@@ -2578,35 +2578,35 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>PE CAMPO LINDO</t>
+          <t>PE VALLE DE LOS VIENTOS</t>
         </is>
       </c>
       <c r="B47" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C47" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D47" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E47" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F47" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G47" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H47" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I47" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J47" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K47" t="n">
         <v>0</v>

</xml_diff>